<commit_message>
modify git ignore and file system
</commit_message>
<xml_diff>
--- a/GanttChart8_26.xlsx
+++ b/GanttChart8_26.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fb53c42262f166b/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fb53c42262f166b/Desktop/Hardware-Security/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="8_{5006A22D-06C8-4681-9ABD-4996206A56AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{246571F2-373C-4DFC-A983-F2EB0CF551DD}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="8_{5006A22D-06C8-4681-9ABD-4996206A56AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99187E0E-F817-45FE-8DC8-8B35B1F1942A}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>ACTIVITY</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Side Channel Processing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1064,10 +1067,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO30"/>
+  <dimension ref="A1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="54" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="63" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="BY8" sqref="BY8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.69921875" defaultRowHeight="29.95" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1331,16 +1334,16 @@
         <v>1</v>
       </c>
       <c r="D5" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E5" s="7">
         <v>1</v>
       </c>
       <c r="F5" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G5" s="8">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="H5" s="18"/>
       <c r="AN5" s="23"/>
@@ -1389,7 +1392,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="8">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="H6" s="18"/>
       <c r="AN6" s="23"/>
@@ -1429,16 +1432,16 @@
         <v>2</v>
       </c>
       <c r="D7" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E7" s="7">
         <v>1</v>
       </c>
       <c r="F7" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G7" s="8">
-        <v>0.15</v>
+        <v>0.7</v>
       </c>
       <c r="AN7" s="23"/>
       <c r="AO7" s="23"/>
@@ -1486,7 +1489,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="8">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="AN8" s="23"/>
       <c r="AO8" s="23"/>
@@ -1525,16 +1528,16 @@
         <v>2</v>
       </c>
       <c r="D9" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E9" s="7">
         <v>2</v>
       </c>
       <c r="F9" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G9" s="8">
-        <v>0.35</v>
+        <v>0.9</v>
       </c>
       <c r="AN9" s="23"/>
       <c r="AO9" s="23"/>
@@ -1582,7 +1585,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="8">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AN10" s="23"/>
       <c r="AO10" s="23"/>
@@ -1621,16 +1624,16 @@
         <v>4</v>
       </c>
       <c r="D11" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11" s="7">
         <v>2</v>
       </c>
       <c r="G11" s="8">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="AN11" s="23"/>
       <c r="AO11" s="23"/>
@@ -1666,13 +1669,13 @@
         <v>25</v>
       </c>
       <c r="C12" s="7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D12" s="7">
         <v>5</v>
       </c>
       <c r="E12" s="7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F12" s="7">
         <v>5</v>
@@ -1714,13 +1717,13 @@
         <v>30</v>
       </c>
       <c r="C13" s="7">
+        <v>6</v>
+      </c>
+      <c r="D13" s="7">
         <v>5</v>
       </c>
-      <c r="D13" s="7">
-        <v>4</v>
-      </c>
       <c r="E13" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F13" s="7">
         <v>4</v>
@@ -1870,7 +1873,7 @@
         <v>25</v>
       </c>
       <c r="G16" s="8">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AN16" s="23"/>
       <c r="AO16" s="23"/>
@@ -1901,7 +1904,7 @@
       <c r="BN16" s="23"/>
       <c r="BO16" s="23"/>
     </row>
-    <row r="17" spans="2:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
         <v>40</v>
       </c>
@@ -1949,24 +1952,24 @@
       <c r="BN17" s="23"/>
       <c r="BO17" s="23"/>
     </row>
-    <row r="18" spans="2:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" s="7">
         <v>2</v>
       </c>
       <c r="E18" s="7">
+        <v>2</v>
+      </c>
+      <c r="F18" s="7">
+        <v>3</v>
+      </c>
+      <c r="G18" s="8">
         <v>1</v>
-      </c>
-      <c r="F18" s="7">
-        <v>2</v>
-      </c>
-      <c r="G18" s="8">
-        <v>0.8</v>
       </c>
       <c r="AN18" s="23"/>
       <c r="AO18" s="23"/>
@@ -1997,7 +2000,7 @@
       <c r="BN18" s="23"/>
       <c r="BO18" s="23"/>
     </row>
-    <row r="19" spans="2:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="6" t="s">
         <v>36</v>
       </c>
@@ -2014,7 +2017,7 @@
         <v>3</v>
       </c>
       <c r="G19" s="8">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="AN19" s="23"/>
       <c r="AO19" s="23"/>
@@ -2045,7 +2048,7 @@
       <c r="BN19" s="23"/>
       <c r="BO19" s="23"/>
     </row>
-    <row r="20" spans="2:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="6" t="s">
         <v>37</v>
       </c>
@@ -2062,7 +2065,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="8">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AN20" s="23"/>
       <c r="AO20" s="23"/>
@@ -2093,7 +2096,7 @@
       <c r="BN20" s="23"/>
       <c r="BO20" s="23"/>
     </row>
-    <row r="21" spans="2:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="6" t="s">
         <v>38</v>
       </c>
@@ -2110,7 +2113,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="8">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="AN21" s="23"/>
       <c r="AO21" s="23"/>
@@ -2141,18 +2144,18 @@
       <c r="BN21" s="23"/>
       <c r="BO21" s="23"/>
     </row>
-    <row r="22" spans="2:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D22" s="7">
         <v>9</v>
       </c>
       <c r="E22" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F22" s="7">
         <v>9</v>
@@ -2189,7 +2192,7 @@
       <c r="BN22" s="23"/>
       <c r="BO22" s="23"/>
     </row>
-    <row r="23" spans="2:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="6" t="s">
         <v>41</v>
       </c>
@@ -2237,7 +2240,10 @@
       <c r="BN23" s="23"/>
       <c r="BO23" s="23"/>
     </row>
-    <row r="24" spans="2:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
       <c r="B24" s="6" t="s">
         <v>1</v>
       </c>
@@ -2285,7 +2291,7 @@
       <c r="BN24" s="23"/>
       <c r="BO24" s="23"/>
     </row>
-    <row r="25" spans="2:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
         <v>2</v>
       </c>
@@ -2333,7 +2339,7 @@
       <c r="BN25" s="23"/>
       <c r="BO25" s="23"/>
     </row>
-    <row r="26" spans="2:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6" t="s">
         <v>3</v>
       </c>
@@ -2381,7 +2387,7 @@
       <c r="BN26" s="23"/>
       <c r="BO26" s="23"/>
     </row>
-    <row r="27" spans="2:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
         <v>4</v>
       </c>
@@ -2429,7 +2435,7 @@
       <c r="BN27" s="23"/>
       <c r="BO27" s="23"/>
     </row>
-    <row r="28" spans="2:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="6" t="s">
         <v>5</v>
       </c>
@@ -2477,7 +2483,7 @@
       <c r="BN28" s="23"/>
       <c r="BO28" s="23"/>
     </row>
-    <row r="29" spans="2:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="6" t="s">
         <v>6</v>
       </c>
@@ -2525,7 +2531,7 @@
       <c r="BN29" s="23"/>
       <c r="BO29" s="23"/>
     </row>
-    <row r="30" spans="2:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:67" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="6" t="s">
         <v>7</v>
       </c>

</xml_diff>